<commit_message>
Updated to include chatbot
</commit_message>
<xml_diff>
--- a/assets/exceldata.xlsx
+++ b/assets/exceldata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bencahill/Documents/python_progs/Prioritising_Tool/PriorTool/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBCA8C28-B2CC-EC48-B714-F0E9AC403627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFABF4EB-5992-3C4D-9CD6-CD716E9EF6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14980" yWindow="760" windowWidth="19580" windowHeight="20620" xr2:uid="{A8BEBEA9-D1E6-634C-884B-3ACC2F953EB0}"/>
+    <workbookView xWindow="11360" yWindow="760" windowWidth="19580" windowHeight="20620" xr2:uid="{A8BEBEA9-D1E6-634C-884B-3ACC2F953EB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76784108-58B2-6945-B52F-A78989885E15}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E36" sqref="A33:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>